<commit_message>
perubahan terakhir terkait persedian, belum selesai
</commit_message>
<xml_diff>
--- a/storage/data/data.xlsx
+++ b/storage/data/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="profile" sheetId="1" state="visible" r:id="rId2"/>
@@ -75,6 +75,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Jika produk ada paket gunakan sesui no dengan pemisah menggunakan ( json )
 Contoh :
@@ -94,6 +95,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">status disi aktif dan nonaktif</t>
         </r>
@@ -129,6 +131,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Gajii diambil harian</t>
         </r>
@@ -177,6 +180,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Role harus di antara
  Kasir, Bagian Keuangan, Bagian SDM, Bagian Produksi</t>
@@ -188,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="210">
   <si>
     <t xml:space="preserve">Nama</t>
   </si>
@@ -822,21 +826,6 @@
   </si>
   <si>
     <t xml:space="preserve">SALDO AWAL PERLENGKAPAN (BUKU)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CUP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KERTAS CHICKEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAWANG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ES</t>
   </si>
   <si>
     <t xml:space="preserve">Debet</t>
@@ -863,7 +852,7 @@
     <numFmt numFmtId="168" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="169" formatCode="[$Rp-421]* #,##0\ ;\-[$Rp-421]* #,##0\ ;[$Rp-421]* \-#\ ;\ @\ "/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -884,11 +873,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -984,7 +968,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1017,7 +1001,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1041,11 +1025,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1069,7 +1053,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1077,15 +1061,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1133,7 +1113,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.86"/>
@@ -1183,7 +1163,7 @@
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1273,7 +1253,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.24"/>
@@ -13808,13 +13788,13 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="43.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="43.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13923,7 +13903,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.79"/>
   </cols>
@@ -14005,7 +13985,7 @@
       <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.72"/>
@@ -14487,13 +14467,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K97"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.98"/>
@@ -15132,1366 +15112,6 @@
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D30" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E30" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="F30" s="9" t="n">
-        <v>400000</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D31" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E31" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F31" s="9" t="n">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C32" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D32" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E32" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F32" s="9" t="n">
-        <v>58000</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D33" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E33" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F33" s="9" t="n">
-        <v>79000</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D34" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E34" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F34" s="9" t="n">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C35" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D35" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E35" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F35" s="9" t="n">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C36" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D36" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E36" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F36" s="9" t="n">
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D37" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E37" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="F37" s="9" t="n">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="n">
-        <v>37</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D38" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E38" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F38" s="23" t="n">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C39" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D39" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E39" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="F39" s="9" t="n">
-        <v>21000</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C40" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D40" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E40" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F40" s="9" t="n">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D41" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E41" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F41" s="9" t="n">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="n">
-        <v>41</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D42" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E42" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F42" s="9" t="n">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C43" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D43" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E43" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F43" s="9" t="n">
-        <v>54000</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="n">
-        <v>43</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D44" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E44" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F44" s="9" t="n">
-        <v>34000</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="n">
-        <v>44</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D45" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E45" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F45" s="9" t="n">
-        <v>53000</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D46" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E46" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F46" s="9" t="n">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C47" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D47" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E47" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F47" s="9" t="n">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="n">
-        <v>47</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C48" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D48" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E48" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F48" s="9" t="n">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C49" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D49" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E49" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F49" s="9" t="n">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="n">
-        <v>49</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C50" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D50" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E50" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="F50" s="9" t="n">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C51" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D51" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E51" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F51" s="9" t="n">
-        <v>63000</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C52" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D52" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E52" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F52" s="9" t="n">
-        <v>39000</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="n">
-        <v>52</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C53" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D53" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E53" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F53" s="9" t="n">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="n">
-        <v>53</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C54" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D54" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E54" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F54" s="9" t="n">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5" t="n">
-        <v>54</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C55" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D55" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E55" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F55" s="9" t="n">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="n">
-        <v>55</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C56" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D56" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E56" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F56" s="9" t="n">
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="n">
-        <v>56</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C57" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D57" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E57" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="F57" s="9" t="n">
-        <v>27000</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="n">
-        <v>57</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C58" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D58" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E58" s="5" t="n">
-        <v>23</v>
-      </c>
-      <c r="F58" s="9" t="n">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="n">
-        <v>58</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C59" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D59" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E59" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F59" s="9" t="n">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="n">
-        <v>59</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C60" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D60" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E60" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="F60" s="9" t="n">
-        <v>21000</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5" t="n">
-        <v>60</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C61" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D61" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E61" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F61" s="9" t="n">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="n">
-        <v>61</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C62" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D62" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E62" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F62" s="9" t="n">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="n">
-        <v>62</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C63" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D63" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E63" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F63" s="9" t="n">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="n">
-        <v>63</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C64" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D64" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E64" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F64" s="9" t="n">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="n">
-        <v>64</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C65" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D65" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E65" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F65" s="9" t="n">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="n">
-        <v>65</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C66" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D66" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E66" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F66" s="9" t="n">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="n">
-        <v>66</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C67" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D67" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E67" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F67" s="9" t="n">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5" t="n">
-        <v>67</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C68" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D68" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E68" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F68" s="9" t="n">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="n">
-        <v>68</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C69" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D69" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E69" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F69" s="9" t="n">
-        <v>12500</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="n">
-        <v>69</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C70" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D70" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E70" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F70" s="9" t="n">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5" t="n">
-        <v>70</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C71" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D71" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E71" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F71" s="9" t="n">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5" t="n">
-        <v>71</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C72" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D72" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E72" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F72" s="9" t="n">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5" t="n">
-        <v>72</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C73" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D73" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E73" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="F73" s="9" t="n">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="n">
-        <v>73</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C74" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D74" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E74" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F74" s="9" t="n">
-        <v>52500</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5" t="n">
-        <v>74</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C75" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D75" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E75" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="F75" s="9" t="n">
-        <v>19500</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="5" t="n">
-        <v>75</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C76" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D76" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E76" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F76" s="9" t="n">
-        <v>79000</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5" t="n">
-        <v>76</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C77" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D77" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E77" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="F77" s="9" t="n">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="5" t="n">
-        <v>77</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C78" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D78" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E78" s="5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F78" s="9" t="n">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="5" t="n">
-        <v>78</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C79" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D79" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E79" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="F79" s="9" t="n">
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="5" t="n">
-        <v>79</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C80" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D80" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E80" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="F80" s="9" t="n">
-        <v>27000</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="5" t="n">
-        <v>80</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C81" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D81" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E81" s="5" t="n">
-        <v>23</v>
-      </c>
-      <c r="F81" s="9" t="n">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="5" t="n">
-        <v>81</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C82" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D82" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E82" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="F82" s="9" t="n">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="5" t="n">
-        <v>82</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C83" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D83" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E83" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F83" s="9" t="n">
-        <v>24000</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="5" t="n">
-        <v>83</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C84" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D84" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E84" s="5" t="n">
-        <v>19</v>
-      </c>
-      <c r="F84" s="9" t="n">
-        <v>21000</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="5" t="n">
-        <v>84</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C85" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D85" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E85" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="F85" s="9" t="n">
-        <v>21000</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="5" t="n">
-        <v>85</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C86" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D86" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E86" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F86" s="9" t="n">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="5" t="n">
-        <v>86</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C87" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D87" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E87" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F87" s="9" t="n">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="5" t="n">
-        <v>87</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C88" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D88" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E88" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F88" s="9" t="n">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="5" t="n">
-        <v>88</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C89" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D89" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E89" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F89" s="9" t="n">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="5" t="n">
-        <v>89</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C90" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D90" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E90" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F90" s="9" t="n">
-        <v>51000</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="5" t="n">
-        <v>90</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C91" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D91" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E91" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F91" s="9" t="n">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="5" t="n">
-        <v>91</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C92" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D92" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E92" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F92" s="9" t="n">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="5" t="n">
-        <v>92</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C93" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D93" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E93" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F93" s="9" t="n">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="5" t="n">
-        <v>93</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C94" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D94" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E94" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F94" s="9" t="n">
-        <v>12500</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="5" t="n">
-        <v>94</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C95" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D95" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E95" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F95" s="9" t="n">
-        <v>19000</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="5" t="n">
-        <v>95</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C96" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D96" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E96" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F96" s="9" t="n">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="5" t="n">
-        <v>96</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C97" s="5" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D97" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E97" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F97" s="9" t="n">
-        <v>10000</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -16515,7 +15135,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.4"/>
@@ -16541,23 +15161,23 @@
         <v>96</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="n">
+      <c r="B2" s="23" t="n">
         <v>45658</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="D2" s="25" t="n">
+        <v>208</v>
+      </c>
+      <c r="D2" s="24" t="n">
         <v>1491000</v>
       </c>
       <c r="E2" s="0" t="n">
@@ -16624,7 +15244,7 @@
         <v>45658</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D5" s="9" t="n">
         <v>500000</v>
@@ -16868,7 +15488,7 @@
       <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.58"/>
@@ -17016,11 +15636,11 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="66.41"/>
   </cols>
@@ -17478,7 +16098,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.03"/>
@@ -17913,7 +16533,7 @@
       <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.43"/>
@@ -18055,15 +16675,15 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="22.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="22.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="36.26"/>
   </cols>
   <sheetData>
@@ -18132,7 +16752,7 @@
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="54.18"/>
   </cols>
@@ -18616,7 +17236,7 @@
       <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.64"/>
@@ -18748,7 +17368,7 @@
       <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.31"/>

</xml_diff>

<commit_message>
perbaiki input edit transaksi
</commit_message>
<xml_diff>
--- a/storage/data/data.xlsx
+++ b/storage/data/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="profile" sheetId="1" state="visible" r:id="rId2"/>
@@ -747,14 +747,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot; Rp&quot;* #,##0.00\ ;&quot;-Rp&quot;* #,##0.00\ ;&quot; Rp&quot;* \-#\ ;@\ "/>
     <numFmt numFmtId="166" formatCode="[$Rp-421]* #,##0\ ;\-[$Rp-421]* #,##0\ ;[$Rp-421]* \-#\ ;@\ "/>
     <numFmt numFmtId="167" formatCode="&quot; Rp&quot;* #,##0\ ;&quot;-Rp&quot;* #,##0\ ;&quot; Rp&quot;* \-#\ ;@\ "/>
     <numFmt numFmtId="168" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="169" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="170" formatCode="[$Rp-421]* #,##0\ ;\-[$Rp-421]* #,##0\ ;[$Rp-421]* \-#\ ;@\ "/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -875,7 +874,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -976,15 +975,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1045,7 +1040,7 @@
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.86"/>
@@ -1091,11 +1086,11 @@
   </sheetPr>
   <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.31"/>
@@ -3304,13 +3299,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -3321,6 +3316,39 @@
       </c>
       <c r="C1" s="0" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3342,10 +3370,10 @@
   <dimension ref="A1:L559"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.24"/>
@@ -15876,11 +15904,11 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.9"/>
@@ -15989,11 +16017,11 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.04"/>
   </cols>
@@ -16031,7 +16059,7 @@
       <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.72"/>
@@ -16519,7 +16547,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.98"/>
@@ -16955,7 +16983,7 @@
       <c r="E20" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="F20" s="27" t="n">
+      <c r="F20" s="2" t="n">
         <v>24000</v>
       </c>
       <c r="J20" s="3"/>
@@ -16977,7 +17005,7 @@
       <c r="E21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="F21" s="27" t="n">
+      <c r="F21" s="2" t="n">
         <v>16000</v>
       </c>
       <c r="J21" s="3"/>
@@ -16999,7 +17027,7 @@
       <c r="E22" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="F22" s="27" t="n">
+      <c r="F22" s="2" t="n">
         <v>9000</v>
       </c>
       <c r="J22" s="3"/>
@@ -17021,7 +17049,7 @@
       <c r="E23" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="F23" s="27" t="n">
+      <c r="F23" s="2" t="n">
         <v>18000</v>
       </c>
       <c r="J23" s="3"/>
@@ -17043,7 +17071,7 @@
       <c r="E24" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="F24" s="27" t="n">
+      <c r="F24" s="2" t="n">
         <v>7000</v>
       </c>
       <c r="J24" s="3"/>
@@ -17065,7 +17093,7 @@
       <c r="E25" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="F25" s="27" t="n">
+      <c r="F25" s="2" t="n">
         <v>15000</v>
       </c>
       <c r="J25" s="3"/>
@@ -17087,7 +17115,7 @@
       <c r="E26" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="F26" s="27" t="n">
+      <c r="F26" s="2" t="n">
         <v>6000</v>
       </c>
       <c r="J26" s="3"/>
@@ -17109,7 +17137,7 @@
       <c r="E27" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="F27" s="27" t="n">
+      <c r="F27" s="2" t="n">
         <v>5000</v>
       </c>
       <c r="J27" s="3"/>
@@ -17131,7 +17159,7 @@
       <c r="E28" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="F28" s="27" t="n">
+      <c r="F28" s="2" t="n">
         <v>5000</v>
       </c>
       <c r="J28" s="3"/>
@@ -17153,7 +17181,7 @@
       <c r="E29" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="F29" s="27" t="n">
+      <c r="F29" s="2" t="n">
         <v>18000</v>
       </c>
       <c r="J29" s="3"/>
@@ -17335,7 +17363,7 @@
       <c r="E38" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="F38" s="28" t="n">
+      <c r="F38" s="27" t="n">
         <v>9000</v>
       </c>
     </row>
@@ -18541,7 +18569,7 @@
       <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.79"/>
@@ -18868,7 +18896,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.4"/>
@@ -18904,13 +18932,13 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="n">
+      <c r="B2" s="28" t="n">
         <v>45658</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="D2" s="30" t="n">
+      <c r="D2" s="29" t="n">
         <v>1491000</v>
       </c>
       <c r="E2" s="0" t="n">
@@ -18945,7 +18973,7 @@
       <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.58"/>
@@ -19113,10 +19141,10 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.43"/>
@@ -19485,11 +19513,11 @@
   </sheetPr>
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B91" activeCellId="0" sqref="B91"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.08"/>
   </cols>
@@ -21029,7 +21057,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.03"/>
@@ -21461,10 +21489,10 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.43"/>
@@ -21632,10 +21660,10 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.17"/>
@@ -21745,11 +21773,11 @@
   </sheetPr>
   <dimension ref="A1:G451"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D454" activeCellId="0" sqref="D454"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="54.18"/>
   </cols>
@@ -26743,7 +26771,7 @@
       <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.64"/>

</xml_diff>